<commit_message>
First functionality of project data interface
</commit_message>
<xml_diff>
--- a/data/gebouwprofielen.xlsx
+++ b/data/gebouwprofielen.xlsx
@@ -435,7 +435,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>110</v>
+        <v>999</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -468,7 +468,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>210</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>